<commit_message>
end of EMI file
</commit_message>
<xml_diff>
--- a/MasterDegree_StudyPlan.xlsx
+++ b/MasterDegree_StudyPlan.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Michael\GitHub\Repo\Master-courses\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{73250FE8-FB70-4537-B6B8-3C5C42E8AE38}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0725186E-AF3B-4780-B6BD-5AEFCAF8ABB8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{9CCEDFCE-005C-40C2-92E8-4E076261F21E}"/>
   </bookViews>
@@ -480,7 +480,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="32">
+  <cellXfs count="36">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -498,28 +498,16 @@
     <xf numFmtId="0" fontId="5" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="1" fillId="3" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="1" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -529,9 +517,6 @@
     <xf numFmtId="0" fontId="8" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="4" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="1" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -547,9 +532,6 @@
     <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="3" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="8" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
@@ -569,6 +551,36 @@
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="2" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="4" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="2" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="2" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="3" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="3" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
@@ -576,6 +588,61 @@
     <cellStyle name="Normale" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="13">
+    <dxf>
+      <font>
+        <b/>
+        <strike val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="12"/>
+        <color theme="1"/>
+        <name val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </font>
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <border diagonalUp="0" diagonalDown="0" outline="0">
+        <left/>
+        <right style="thin">
+          <color auto="1"/>
+        </right>
+        <top style="thin">
+          <color auto="1"/>
+        </top>
+        <bottom style="thin">
+          <color auto="1"/>
+        </bottom>
+      </border>
+    </dxf>
+    <dxf>
+      <font>
+        <strike val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="12"/>
+        <color theme="1"/>
+        <name val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </font>
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <border diagonalUp="0" diagonalDown="0" outline="0">
+        <left/>
+        <right style="thin">
+          <color auto="1"/>
+        </right>
+        <top style="thin">
+          <color auto="1"/>
+        </top>
+        <bottom style="thin">
+          <color auto="1"/>
+        </bottom>
+      </border>
+    </dxf>
     <dxf>
       <font>
         <strike val="0"/>
@@ -771,74 +838,6 @@
         <left style="thin">
           <color auto="1"/>
         </left>
-        <right style="thin">
-          <color auto="1"/>
-        </right>
-        <top style="thin">
-          <color auto="1"/>
-        </top>
-        <bottom style="thin">
-          <color auto="1"/>
-        </bottom>
-        <vertical style="thin">
-          <color auto="1"/>
-        </vertical>
-        <horizontal style="thin">
-          <color auto="1"/>
-        </horizontal>
-      </border>
-    </dxf>
-    <dxf>
-      <font>
-        <strike val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="12"/>
-        <color theme="1"/>
-        <name val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </font>
-      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-      <border diagonalUp="0" diagonalDown="0">
-        <left style="thin">
-          <color auto="1"/>
-        </left>
-        <right style="thin">
-          <color auto="1"/>
-        </right>
-        <top style="thin">
-          <color auto="1"/>
-        </top>
-        <bottom style="thin">
-          <color auto="1"/>
-        </bottom>
-        <vertical style="thin">
-          <color auto="1"/>
-        </vertical>
-        <horizontal style="thin">
-          <color auto="1"/>
-        </horizontal>
-      </border>
-    </dxf>
-    <dxf>
-      <font>
-        <strike val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="12"/>
-        <color theme="1"/>
-        <name val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </font>
-      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-      <border diagonalUp="0" diagonalDown="0">
-        <left/>
         <right style="thin">
           <color auto="1"/>
         </right>
@@ -1059,17 +1058,17 @@
 <table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="2" xr:uid="{F8406AB2-104B-4585-87AD-689DBD0111DE}" name="Tabella2" displayName="Tabella2" ref="A4:H21" totalsRowShown="0" headerRowDxfId="12" dataDxfId="10" headerRowBorderDxfId="11" tableBorderDxfId="9" totalsRowBorderDxfId="8">
   <autoFilter ref="A4:H21" xr:uid="{F8406AB2-104B-4585-87AD-689DBD0111DE}"/>
   <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A5:H21">
-    <sortCondition ref="E4:E21"/>
+    <sortCondition ref="H4:H21"/>
   </sortState>
   <tableColumns count="8">
-    <tableColumn id="1" xr3:uid="{030FDB74-6B11-48DD-A02F-DBE88F27EB4F}" name="Course" dataDxfId="7"/>
-    <tableColumn id="2" xr3:uid="{B359D6B6-2405-42B9-80DD-CF995BBC33B1}" name="Professor" dataDxfId="6"/>
-    <tableColumn id="3" xr3:uid="{C2D716C1-F051-48A0-9247-54C3A56FBE0F}" name="Type" dataDxfId="5"/>
-    <tableColumn id="4" xr3:uid="{8BF37862-6EAD-47FB-BE66-14C3DACF2F7C}" name="Examination Method" dataDxfId="4"/>
-    <tableColumn id="9" xr3:uid="{65F15266-CF73-4302-BA82-7B61D4442B2D}" name="Year" dataDxfId="3"/>
-    <tableColumn id="5" xr3:uid="{0C60A9B7-BB80-49F0-A892-4A29BA4B6C00}" name="Semester" dataDxfId="2"/>
-    <tableColumn id="6" xr3:uid="{AF4E938B-3794-456A-BD30-86A1BEC96769}" name="ETCS" dataDxfId="1"/>
-    <tableColumn id="7" xr3:uid="{F555908D-5B70-4AEA-B0EB-22543AA6A3AF}" name="PASSED" dataDxfId="0"/>
+    <tableColumn id="1" xr3:uid="{030FDB74-6B11-48DD-A02F-DBE88F27EB4F}" name="Course" dataDxfId="0"/>
+    <tableColumn id="2" xr3:uid="{B359D6B6-2405-42B9-80DD-CF995BBC33B1}" name="Professor" dataDxfId="1"/>
+    <tableColumn id="3" xr3:uid="{C2D716C1-F051-48A0-9247-54C3A56FBE0F}" name="Type" dataDxfId="7"/>
+    <tableColumn id="4" xr3:uid="{8BF37862-6EAD-47FB-BE66-14C3DACF2F7C}" name="Examination Method" dataDxfId="6"/>
+    <tableColumn id="9" xr3:uid="{65F15266-CF73-4302-BA82-7B61D4442B2D}" name="Year" dataDxfId="5"/>
+    <tableColumn id="5" xr3:uid="{0C60A9B7-BB80-49F0-A892-4A29BA4B6C00}" name="Semester" dataDxfId="4"/>
+    <tableColumn id="6" xr3:uid="{AF4E938B-3794-456A-BD30-86A1BEC96769}" name="ETCS" dataDxfId="3"/>
+    <tableColumn id="7" xr3:uid="{F555908D-5B70-4AEA-B0EB-22543AA6A3AF}" name="PASSED" dataDxfId="2"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -1374,8 +1373,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{89E4B725-BD0D-4291-9550-3225AF05D5FC}">
   <dimension ref="A1:K22"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A9" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="D13" sqref="D13"/>
+    <sheetView tabSelected="1" topLeftCell="A7" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="K9" sqref="K9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1394,36 +1393,36 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:11" x14ac:dyDescent="0.3">
-      <c r="A1" s="31" t="s">
+      <c r="A1" s="25" t="s">
         <v>41</v>
       </c>
-      <c r="B1" s="31"/>
-      <c r="C1" s="31"/>
-      <c r="D1" s="31"/>
-      <c r="E1" s="31"/>
-      <c r="F1" s="31"/>
-      <c r="G1" s="31"/>
-      <c r="H1" s="31"/>
+      <c r="B1" s="25"/>
+      <c r="C1" s="25"/>
+      <c r="D1" s="25"/>
+      <c r="E1" s="25"/>
+      <c r="F1" s="25"/>
+      <c r="G1" s="25"/>
+      <c r="H1" s="25"/>
     </row>
     <row r="2" spans="1:11" x14ac:dyDescent="0.3">
-      <c r="A2" s="31"/>
-      <c r="B2" s="31"/>
-      <c r="C2" s="31"/>
-      <c r="D2" s="31"/>
-      <c r="E2" s="31"/>
-      <c r="F2" s="31"/>
-      <c r="G2" s="31"/>
-      <c r="H2" s="31"/>
+      <c r="A2" s="25"/>
+      <c r="B2" s="25"/>
+      <c r="C2" s="25"/>
+      <c r="D2" s="25"/>
+      <c r="E2" s="25"/>
+      <c r="F2" s="25"/>
+      <c r="G2" s="25"/>
+      <c r="H2" s="25"/>
     </row>
     <row r="3" spans="1:11" x14ac:dyDescent="0.3">
-      <c r="A3" s="31"/>
-      <c r="B3" s="31"/>
-      <c r="C3" s="31"/>
-      <c r="D3" s="31"/>
-      <c r="E3" s="31"/>
-      <c r="F3" s="31"/>
-      <c r="G3" s="31"/>
-      <c r="H3" s="31"/>
+      <c r="A3" s="25"/>
+      <c r="B3" s="25"/>
+      <c r="C3" s="25"/>
+      <c r="D3" s="25"/>
+      <c r="E3" s="25"/>
+      <c r="F3" s="25"/>
+      <c r="G3" s="25"/>
+      <c r="H3" s="25"/>
     </row>
     <row r="4" spans="1:11" ht="26.4" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A4" s="4" t="s">
@@ -1450,443 +1449,441 @@
       <c r="H4" s="6" t="s">
         <v>57</v>
       </c>
-      <c r="J4" s="17" t="s">
+    </row>
+    <row r="5" spans="1:11" ht="32.4" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A5" s="28" t="s">
+        <v>54</v>
+      </c>
+      <c r="B5" s="7" t="s">
+        <v>51</v>
+      </c>
+      <c r="C5" s="7" t="s">
+        <v>53</v>
+      </c>
+      <c r="D5" s="7" t="s">
+        <v>10</v>
+      </c>
+      <c r="E5" s="7">
+        <v>1</v>
+      </c>
+      <c r="F5" s="7">
+        <v>1</v>
+      </c>
+      <c r="G5" s="7">
+        <v>6</v>
+      </c>
+      <c r="H5" s="21" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="6" spans="1:11" ht="39.6" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A6" s="28" t="s">
+        <v>0</v>
+      </c>
+      <c r="B6" s="7" t="s">
+        <v>1</v>
+      </c>
+      <c r="C6" s="7" t="s">
+        <v>2</v>
+      </c>
+      <c r="D6" s="7" t="s">
+        <v>10</v>
+      </c>
+      <c r="E6" s="7">
+        <v>1</v>
+      </c>
+      <c r="F6" s="7">
+        <v>1</v>
+      </c>
+      <c r="G6" s="7">
+        <v>6</v>
+      </c>
+      <c r="H6" s="21" t="s">
+        <v>33</v>
+      </c>
+      <c r="I6" s="2"/>
+    </row>
+    <row r="7" spans="1:11" ht="52.2" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A7" s="29" t="s">
+        <v>16</v>
+      </c>
+      <c r="B7" s="7" t="s">
+        <v>17</v>
+      </c>
+      <c r="C7" s="7" t="s">
+        <v>12</v>
+      </c>
+      <c r="D7" s="7" t="s">
+        <v>45</v>
+      </c>
+      <c r="E7" s="7">
+        <v>1</v>
+      </c>
+      <c r="F7" s="7">
+        <v>1</v>
+      </c>
+      <c r="G7" s="7">
+        <v>6</v>
+      </c>
+      <c r="H7" s="21" t="s">
+        <v>33</v>
+      </c>
+      <c r="J7" s="16"/>
+      <c r="K7" s="2"/>
+    </row>
+    <row r="8" spans="1:11" ht="60" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A8" s="29" t="s">
+        <v>40</v>
+      </c>
+      <c r="B8" s="7" t="s">
+        <v>3</v>
+      </c>
+      <c r="C8" s="7" t="s">
+        <v>2</v>
+      </c>
+      <c r="D8" s="8" t="s">
+        <v>10</v>
+      </c>
+      <c r="E8" s="7">
+        <v>1</v>
+      </c>
+      <c r="F8" s="7">
+        <v>1</v>
+      </c>
+      <c r="G8" s="7">
+        <v>6</v>
+      </c>
+      <c r="H8" s="21"/>
+      <c r="J8" s="18"/>
+    </row>
+    <row r="9" spans="1:11" ht="59.4" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A9" s="30" t="s">
+        <v>18</v>
+      </c>
+      <c r="B9" s="14" t="s">
+        <v>19</v>
+      </c>
+      <c r="C9" s="14" t="s">
+        <v>12</v>
+      </c>
+      <c r="D9" s="15" t="s">
+        <v>55</v>
+      </c>
+      <c r="E9" s="14">
+        <v>1</v>
+      </c>
+      <c r="F9" s="14">
+        <v>1</v>
+      </c>
+      <c r="G9" s="14">
+        <v>6</v>
+      </c>
+      <c r="H9" s="22"/>
+      <c r="I9" s="2"/>
+      <c r="J9" s="17" t="s">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="10" spans="1:11" ht="43.2" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A10" s="31" t="s">
+        <v>39</v>
+      </c>
+      <c r="B10" s="26" t="s">
+        <v>9</v>
+      </c>
+      <c r="C10" s="26" t="s">
+        <v>2</v>
+      </c>
+      <c r="D10" s="26" t="s">
+        <v>10</v>
+      </c>
+      <c r="E10" s="26">
+        <v>1</v>
+      </c>
+      <c r="F10" s="26">
+        <v>2</v>
+      </c>
+      <c r="G10" s="26">
+        <v>6</v>
+      </c>
+      <c r="H10" s="27"/>
+      <c r="J10" s="13" t="s">
         <v>52</v>
       </c>
     </row>
-    <row r="5" spans="1:11" ht="32.4" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A5" s="7" t="s">
-        <v>54</v>
-      </c>
-      <c r="B5" s="8" t="s">
-        <v>51</v>
-      </c>
-      <c r="C5" s="8" t="s">
-        <v>53</v>
-      </c>
-      <c r="D5" s="8" t="s">
-        <v>10</v>
-      </c>
-      <c r="E5" s="8">
+    <row r="11" spans="1:11" ht="59.4" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A11" s="32" t="s">
+        <v>14</v>
+      </c>
+      <c r="B11" s="26" t="s">
+        <v>15</v>
+      </c>
+      <c r="C11" s="26" t="s">
+        <v>12</v>
+      </c>
+      <c r="D11" s="26" t="s">
+        <v>60</v>
+      </c>
+      <c r="E11" s="26">
         <v>1</v>
       </c>
-      <c r="F5" s="8">
+      <c r="F11" s="26">
+        <v>2</v>
+      </c>
+      <c r="G11" s="26">
+        <v>6</v>
+      </c>
+      <c r="H11" s="27"/>
+    </row>
+    <row r="12" spans="1:11" ht="39.6" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A12" s="31" t="s">
+        <v>26</v>
+      </c>
+      <c r="B12" s="26" t="s">
+        <v>28</v>
+      </c>
+      <c r="C12" s="26" t="s">
+        <v>27</v>
+      </c>
+      <c r="D12" s="26" t="s">
+        <v>45</v>
+      </c>
+      <c r="E12" s="26">
         <v>1</v>
       </c>
-      <c r="G5" s="8">
-        <v>6</v>
-      </c>
-      <c r="H5" s="27" t="s">
-        <v>33</v>
-      </c>
-    </row>
-    <row r="6" spans="1:11" ht="39.6" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A6" s="7" t="s">
-        <v>0</v>
-      </c>
-      <c r="B6" s="8" t="s">
-        <v>1</v>
-      </c>
-      <c r="C6" s="8" t="s">
+      <c r="F12" s="26">
         <v>2</v>
       </c>
-      <c r="D6" s="8" t="s">
-        <v>10</v>
-      </c>
-      <c r="E6" s="8">
-        <v>1</v>
-      </c>
-      <c r="F6" s="8">
-        <v>1</v>
-      </c>
-      <c r="G6" s="8">
-        <v>6</v>
-      </c>
-      <c r="H6" s="27" t="s">
-        <v>33</v>
-      </c>
-      <c r="I6" s="2"/>
-      <c r="J6" s="22" t="s">
-        <v>56</v>
-      </c>
-    </row>
-    <row r="7" spans="1:11" ht="52.2" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A7" s="9" t="s">
-        <v>40</v>
-      </c>
-      <c r="B7" s="8" t="s">
-        <v>3</v>
-      </c>
-      <c r="C7" s="8" t="s">
-        <v>2</v>
-      </c>
-      <c r="D7" s="10" t="s">
-        <v>10</v>
-      </c>
-      <c r="E7" s="8">
-        <v>1</v>
-      </c>
-      <c r="F7" s="8">
-        <v>1</v>
-      </c>
-      <c r="G7" s="8">
-        <v>6</v>
-      </c>
-      <c r="H7" s="27"/>
-      <c r="J7" s="21"/>
-      <c r="K7" s="2"/>
-    </row>
-    <row r="8" spans="1:11" ht="48" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A8" s="9" t="s">
-        <v>16</v>
-      </c>
-      <c r="B8" s="8" t="s">
-        <v>17</v>
-      </c>
-      <c r="C8" s="8" t="s">
-        <v>12</v>
-      </c>
-      <c r="D8" s="8" t="s">
-        <v>45</v>
-      </c>
-      <c r="E8" s="8">
-        <v>1</v>
-      </c>
-      <c r="F8" s="8">
-        <v>1</v>
-      </c>
-      <c r="G8" s="8">
-        <v>6</v>
-      </c>
-      <c r="H8" s="27" t="s">
-        <v>33</v>
-      </c>
-      <c r="J8" s="23"/>
-    </row>
-    <row r="9" spans="1:11" ht="52.2" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A9" s="18" t="s">
-        <v>18</v>
-      </c>
-      <c r="B9" s="19" t="s">
-        <v>19</v>
-      </c>
-      <c r="C9" s="19" t="s">
-        <v>12</v>
-      </c>
-      <c r="D9" s="20" t="s">
-        <v>55</v>
-      </c>
-      <c r="E9" s="19">
-        <v>1</v>
-      </c>
-      <c r="F9" s="19">
-        <v>1</v>
-      </c>
-      <c r="G9" s="19">
-        <v>6</v>
-      </c>
-      <c r="H9" s="28"/>
-      <c r="I9" s="2"/>
-      <c r="J9" s="2"/>
-    </row>
-    <row r="10" spans="1:11" ht="43.2" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A10" s="7" t="s">
-        <v>39</v>
-      </c>
-      <c r="B10" s="8" t="s">
-        <v>9</v>
-      </c>
-      <c r="C10" s="8" t="s">
-        <v>2</v>
-      </c>
-      <c r="D10" s="8" t="s">
-        <v>10</v>
-      </c>
-      <c r="E10" s="8">
-        <v>1</v>
-      </c>
-      <c r="F10" s="8">
-        <v>2</v>
-      </c>
-      <c r="G10" s="8">
-        <v>6</v>
-      </c>
-      <c r="H10" s="27"/>
-      <c r="J10" s="2"/>
-    </row>
-    <row r="11" spans="1:11" ht="59.4" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A11" s="9" t="s">
-        <v>14</v>
-      </c>
-      <c r="B11" s="8" t="s">
-        <v>15</v>
-      </c>
-      <c r="C11" s="8" t="s">
-        <v>12</v>
-      </c>
-      <c r="D11" s="8" t="s">
-        <v>60</v>
-      </c>
-      <c r="E11" s="8">
-        <v>1</v>
-      </c>
-      <c r="F11" s="8">
-        <v>2</v>
-      </c>
-      <c r="G11" s="8">
-        <v>6</v>
-      </c>
-      <c r="H11" s="27"/>
-    </row>
-    <row r="12" spans="1:11" ht="39.6" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A12" s="7" t="s">
-        <v>26</v>
-      </c>
-      <c r="B12" s="8" t="s">
-        <v>28</v>
-      </c>
-      <c r="C12" s="8" t="s">
-        <v>27</v>
-      </c>
-      <c r="D12" s="8" t="s">
-        <v>45</v>
-      </c>
-      <c r="E12" s="8">
-        <v>1</v>
-      </c>
-      <c r="F12" s="8">
-        <v>2</v>
-      </c>
-      <c r="G12" s="8">
+      <c r="G12" s="26">
         <v>6</v>
       </c>
       <c r="H12" s="27"/>
       <c r="I12" s="2"/>
     </row>
     <row r="13" spans="1:11" ht="47.4" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A13" s="7" t="s">
+      <c r="A13" s="31" t="s">
         <v>46</v>
       </c>
-      <c r="B13" s="8" t="s">
+      <c r="B13" s="26" t="s">
         <v>48</v>
       </c>
-      <c r="C13" s="8" t="s">
+      <c r="C13" s="26" t="s">
         <v>20</v>
       </c>
-      <c r="D13" s="8" t="s">
+      <c r="D13" s="26" t="s">
         <v>49</v>
       </c>
-      <c r="E13" s="8">
+      <c r="E13" s="26">
         <v>1</v>
       </c>
-      <c r="F13" s="8">
+      <c r="F13" s="26">
         <v>2</v>
       </c>
-      <c r="G13" s="8">
+      <c r="G13" s="26">
         <v>6</v>
       </c>
       <c r="H13" s="27"/>
     </row>
     <row r="14" spans="1:11" ht="57.6" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A14" s="9" t="s">
+      <c r="A14" s="32" t="s">
         <v>47</v>
       </c>
-      <c r="B14" s="8" t="s">
+      <c r="B14" s="26" t="s">
         <v>50</v>
       </c>
-      <c r="C14" s="8" t="s">
+      <c r="C14" s="26" t="s">
         <v>20</v>
       </c>
-      <c r="D14" s="8" t="s">
+      <c r="D14" s="26" t="s">
         <v>10</v>
       </c>
-      <c r="E14" s="8">
+      <c r="E14" s="26">
         <v>1</v>
       </c>
-      <c r="F14" s="8">
+      <c r="F14" s="26">
         <v>2</v>
       </c>
-      <c r="G14" s="8">
+      <c r="G14" s="26">
         <v>6</v>
       </c>
       <c r="H14" s="27"/>
-      <c r="J14" s="26"/>
+      <c r="J14" s="20"/>
     </row>
     <row r="15" spans="1:11" ht="47.4" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A15" s="7" t="s">
+      <c r="A15" s="28" t="s">
         <v>29</v>
       </c>
-      <c r="B15" s="8" t="s">
+      <c r="B15" s="7" t="s">
         <v>9</v>
       </c>
-      <c r="C15" s="8" t="s">
+      <c r="C15" s="7" t="s">
         <v>2</v>
       </c>
-      <c r="D15" s="8" t="s">
+      <c r="D15" s="7" t="s">
         <v>13</v>
       </c>
-      <c r="E15" s="8">
+      <c r="E15" s="7">
         <v>1</v>
       </c>
-      <c r="F15" s="8" t="s">
+      <c r="F15" s="7" t="s">
         <v>35</v>
       </c>
-      <c r="G15" s="8">
+      <c r="G15" s="7">
         <v>3</v>
       </c>
-      <c r="H15" s="27"/>
+      <c r="H15" s="21"/>
     </row>
     <row r="16" spans="1:11" ht="57.6" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A16" s="24" t="s">
+      <c r="A16" s="33" t="s">
         <v>24</v>
       </c>
-      <c r="B16" s="15" t="s">
+      <c r="B16" s="11" t="s">
         <v>25</v>
       </c>
-      <c r="C16" s="15" t="s">
+      <c r="C16" s="11" t="s">
         <v>20</v>
       </c>
-      <c r="D16" s="16" t="s">
+      <c r="D16" s="12" t="s">
         <v>44</v>
       </c>
-      <c r="E16" s="15">
+      <c r="E16" s="11">
         <v>2</v>
       </c>
-      <c r="F16" s="15">
+      <c r="F16" s="11">
         <v>2</v>
       </c>
-      <c r="G16" s="15">
+      <c r="G16" s="11">
         <v>6</v>
       </c>
-      <c r="H16" s="29"/>
-      <c r="J16" s="25" t="s">
+      <c r="H16" s="23"/>
+      <c r="J16" s="19" t="s">
         <v>58</v>
       </c>
       <c r="K16" s="2"/>
     </row>
     <row r="17" spans="1:10" ht="54.6" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A17" s="14" t="s">
+      <c r="A17" s="34" t="s">
         <v>21</v>
       </c>
-      <c r="B17" s="15" t="s">
+      <c r="B17" s="11" t="s">
         <v>22</v>
       </c>
-      <c r="C17" s="15" t="s">
+      <c r="C17" s="11" t="s">
         <v>53</v>
       </c>
-      <c r="D17" s="16" t="s">
+      <c r="D17" s="12" t="s">
         <v>23</v>
       </c>
-      <c r="E17" s="15">
+      <c r="E17" s="11">
         <v>2</v>
       </c>
-      <c r="F17" s="15">
+      <c r="F17" s="11">
         <v>1</v>
       </c>
-      <c r="G17" s="15">
+      <c r="G17" s="11">
         <v>6</v>
       </c>
-      <c r="H17" s="29"/>
-      <c r="I17" s="13"/>
-      <c r="J17" s="25" t="s">
+      <c r="H17" s="23"/>
+      <c r="I17" s="10"/>
+      <c r="J17" s="19" t="s">
         <v>59</v>
       </c>
     </row>
     <row r="18" spans="1:10" ht="48" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A18" s="9" t="s">
+      <c r="A18" s="29" t="s">
         <v>42</v>
       </c>
-      <c r="B18" s="8" t="s">
+      <c r="B18" s="7" t="s">
         <v>11</v>
       </c>
-      <c r="C18" s="8" t="s">
+      <c r="C18" s="7" t="s">
         <v>12</v>
       </c>
-      <c r="D18" s="8" t="s">
+      <c r="D18" s="7" t="s">
         <v>43</v>
       </c>
-      <c r="E18" s="8">
+      <c r="E18" s="7">
         <v>2</v>
       </c>
-      <c r="F18" s="8">
+      <c r="F18" s="7">
         <v>1</v>
       </c>
-      <c r="G18" s="8">
+      <c r="G18" s="7">
         <v>6</v>
       </c>
-      <c r="H18" s="27"/>
+      <c r="H18" s="21"/>
     </row>
     <row r="19" spans="1:10" ht="37.799999999999997" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A19" s="9" t="s">
+      <c r="A19" s="29" t="s">
         <v>34</v>
       </c>
-      <c r="B19" s="8" t="s">
+      <c r="B19" s="7" t="s">
         <v>38</v>
       </c>
-      <c r="C19" s="8" t="s">
+      <c r="C19" s="7" t="s">
         <v>2</v>
       </c>
-      <c r="D19" s="8" t="s">
+      <c r="D19" s="7" t="s">
         <v>33</v>
       </c>
-      <c r="E19" s="8">
+      <c r="E19" s="7">
         <v>2</v>
       </c>
-      <c r="F19" s="8">
+      <c r="F19" s="7">
         <v>1</v>
       </c>
-      <c r="G19" s="8">
+      <c r="G19" s="7">
         <v>3</v>
       </c>
-      <c r="H19" s="27"/>
+      <c r="H19" s="21"/>
     </row>
     <row r="20" spans="1:10" ht="39.6" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A20" s="9" t="s">
+      <c r="A20" s="29" t="s">
         <v>36</v>
       </c>
-      <c r="B20" s="8" t="s">
+      <c r="B20" s="7" t="s">
         <v>38</v>
       </c>
-      <c r="C20" s="8" t="s">
+      <c r="C20" s="7" t="s">
         <v>2</v>
       </c>
-      <c r="D20" s="8" t="s">
+      <c r="D20" s="7" t="s">
         <v>33</v>
       </c>
-      <c r="E20" s="8">
+      <c r="E20" s="7">
         <v>2</v>
       </c>
-      <c r="F20" s="8">
+      <c r="F20" s="7">
         <v>2</v>
       </c>
-      <c r="G20" s="8">
+      <c r="G20" s="7">
         <v>3</v>
       </c>
-      <c r="H20" s="27"/>
+      <c r="H20" s="21"/>
     </row>
     <row r="21" spans="1:10" ht="32.4" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A21" s="11" t="s">
+      <c r="A21" s="35" t="s">
         <v>37</v>
       </c>
-      <c r="B21" s="12" t="s">
+      <c r="B21" s="9" t="s">
         <v>33</v>
       </c>
-      <c r="C21" s="12" t="s">
+      <c r="C21" s="9" t="s">
         <v>2</v>
       </c>
-      <c r="D21" s="12" t="s">
+      <c r="D21" s="9" t="s">
         <v>33</v>
       </c>
-      <c r="E21" s="12">
+      <c r="E21" s="9">
         <v>2</v>
       </c>
-      <c r="F21" s="12" t="s">
+      <c r="F21" s="9" t="s">
         <v>35</v>
       </c>
-      <c r="G21" s="12">
+      <c r="G21" s="9">
         <v>33</v>
       </c>
-      <c r="H21" s="30"/>
+      <c r="H21" s="24"/>
     </row>
     <row r="22" spans="1:10" ht="32.4" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A22" s="1"/>

</xml_diff>

<commit_message>
Start-up and mobile update + general fix
</commit_message>
<xml_diff>
--- a/MasterDegree_StudyPlan.xlsx
+++ b/MasterDegree_StudyPlan.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Michael\GitHub\Repo\Master-courses\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\GitHub\Repo\Master-courses\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0725186E-AF3B-4780-B6BD-5AEFCAF8ABB8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3FE22213-3885-4FD5-A129-6093487175D5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{9CCEDFCE-005C-40C2-92E8-4E076261F21E}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{9CCEDFCE-005C-40C2-92E8-4E076261F21E}"/>
   </bookViews>
   <sheets>
     <sheet name="Foglio1" sheetId="1" r:id="rId1"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="87" uniqueCount="61">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="88" uniqueCount="61">
   <si>
     <t>Computability</t>
   </si>
@@ -550,9 +550,6 @@
     <xf numFmtId="0" fontId="8" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -581,6 +578,9 @@
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="8" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
@@ -588,61 +588,6 @@
     <cellStyle name="Normale" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="13">
-    <dxf>
-      <font>
-        <b/>
-        <strike val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="12"/>
-        <color theme="1"/>
-        <name val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </font>
-      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-      <border diagonalUp="0" diagonalDown="0" outline="0">
-        <left/>
-        <right style="thin">
-          <color auto="1"/>
-        </right>
-        <top style="thin">
-          <color auto="1"/>
-        </top>
-        <bottom style="thin">
-          <color auto="1"/>
-        </bottom>
-      </border>
-    </dxf>
-    <dxf>
-      <font>
-        <strike val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="12"/>
-        <color theme="1"/>
-        <name val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </font>
-      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-      <border diagonalUp="0" diagonalDown="0" outline="0">
-        <left/>
-        <right style="thin">
-          <color auto="1"/>
-        </right>
-        <top style="thin">
-          <color auto="1"/>
-        </top>
-        <bottom style="thin">
-          <color auto="1"/>
-        </bottom>
-      </border>
-    </dxf>
     <dxf>
       <font>
         <strike val="0"/>
@@ -853,6 +798,61 @@
         <horizontal style="thin">
           <color auto="1"/>
         </horizontal>
+      </border>
+    </dxf>
+    <dxf>
+      <font>
+        <strike val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="12"/>
+        <color theme="1"/>
+        <name val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </font>
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <border diagonalUp="0" diagonalDown="0" outline="0">
+        <left/>
+        <right style="thin">
+          <color auto="1"/>
+        </right>
+        <top style="thin">
+          <color auto="1"/>
+        </top>
+        <bottom style="thin">
+          <color auto="1"/>
+        </bottom>
+      </border>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <strike val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="12"/>
+        <color theme="1"/>
+        <name val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </font>
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <border diagonalUp="0" diagonalDown="0" outline="0">
+        <left/>
+        <right style="thin">
+          <color auto="1"/>
+        </right>
+        <top style="thin">
+          <color auto="1"/>
+        </top>
+        <bottom style="thin">
+          <color auto="1"/>
+        </bottom>
       </border>
     </dxf>
     <dxf>
@@ -1061,14 +1061,14 @@
     <sortCondition ref="H4:H21"/>
   </sortState>
   <tableColumns count="8">
-    <tableColumn id="1" xr3:uid="{030FDB74-6B11-48DD-A02F-DBE88F27EB4F}" name="Course" dataDxfId="0"/>
-    <tableColumn id="2" xr3:uid="{B359D6B6-2405-42B9-80DD-CF995BBC33B1}" name="Professor" dataDxfId="1"/>
-    <tableColumn id="3" xr3:uid="{C2D716C1-F051-48A0-9247-54C3A56FBE0F}" name="Type" dataDxfId="7"/>
-    <tableColumn id="4" xr3:uid="{8BF37862-6EAD-47FB-BE66-14C3DACF2F7C}" name="Examination Method" dataDxfId="6"/>
-    <tableColumn id="9" xr3:uid="{65F15266-CF73-4302-BA82-7B61D4442B2D}" name="Year" dataDxfId="5"/>
-    <tableColumn id="5" xr3:uid="{0C60A9B7-BB80-49F0-A892-4A29BA4B6C00}" name="Semester" dataDxfId="4"/>
-    <tableColumn id="6" xr3:uid="{AF4E938B-3794-456A-BD30-86A1BEC96769}" name="ETCS" dataDxfId="3"/>
-    <tableColumn id="7" xr3:uid="{F555908D-5B70-4AEA-B0EB-22543AA6A3AF}" name="PASSED" dataDxfId="2"/>
+    <tableColumn id="1" xr3:uid="{030FDB74-6B11-48DD-A02F-DBE88F27EB4F}" name="Course" dataDxfId="7"/>
+    <tableColumn id="2" xr3:uid="{B359D6B6-2405-42B9-80DD-CF995BBC33B1}" name="Professor" dataDxfId="6"/>
+    <tableColumn id="3" xr3:uid="{C2D716C1-F051-48A0-9247-54C3A56FBE0F}" name="Type" dataDxfId="5"/>
+    <tableColumn id="4" xr3:uid="{8BF37862-6EAD-47FB-BE66-14C3DACF2F7C}" name="Examination Method" dataDxfId="4"/>
+    <tableColumn id="9" xr3:uid="{65F15266-CF73-4302-BA82-7B61D4442B2D}" name="Year" dataDxfId="3"/>
+    <tableColumn id="5" xr3:uid="{0C60A9B7-BB80-49F0-A892-4A29BA4B6C00}" name="Semester" dataDxfId="2"/>
+    <tableColumn id="6" xr3:uid="{AF4E938B-3794-456A-BD30-86A1BEC96769}" name="ETCS" dataDxfId="1"/>
+    <tableColumn id="7" xr3:uid="{F555908D-5B70-4AEA-B0EB-22543AA6A3AF}" name="PASSED" dataDxfId="0"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -1373,8 +1373,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{89E4B725-BD0D-4291-9550-3225AF05D5FC}">
   <dimension ref="A1:K22"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A7" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="K9" sqref="K9"/>
+    <sheetView tabSelected="1" topLeftCell="A11" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="J14" sqref="J14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1393,36 +1393,36 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:11" x14ac:dyDescent="0.3">
-      <c r="A1" s="25" t="s">
+      <c r="A1" s="35" t="s">
         <v>41</v>
       </c>
-      <c r="B1" s="25"/>
-      <c r="C1" s="25"/>
-      <c r="D1" s="25"/>
-      <c r="E1" s="25"/>
-      <c r="F1" s="25"/>
-      <c r="G1" s="25"/>
-      <c r="H1" s="25"/>
+      <c r="B1" s="35"/>
+      <c r="C1" s="35"/>
+      <c r="D1" s="35"/>
+      <c r="E1" s="35"/>
+      <c r="F1" s="35"/>
+      <c r="G1" s="35"/>
+      <c r="H1" s="35"/>
     </row>
     <row r="2" spans="1:11" x14ac:dyDescent="0.3">
-      <c r="A2" s="25"/>
-      <c r="B2" s="25"/>
-      <c r="C2" s="25"/>
-      <c r="D2" s="25"/>
-      <c r="E2" s="25"/>
-      <c r="F2" s="25"/>
-      <c r="G2" s="25"/>
-      <c r="H2" s="25"/>
+      <c r="A2" s="35"/>
+      <c r="B2" s="35"/>
+      <c r="C2" s="35"/>
+      <c r="D2" s="35"/>
+      <c r="E2" s="35"/>
+      <c r="F2" s="35"/>
+      <c r="G2" s="35"/>
+      <c r="H2" s="35"/>
     </row>
     <row r="3" spans="1:11" x14ac:dyDescent="0.3">
-      <c r="A3" s="25"/>
-      <c r="B3" s="25"/>
-      <c r="C3" s="25"/>
-      <c r="D3" s="25"/>
-      <c r="E3" s="25"/>
-      <c r="F3" s="25"/>
-      <c r="G3" s="25"/>
-      <c r="H3" s="25"/>
+      <c r="A3" s="35"/>
+      <c r="B3" s="35"/>
+      <c r="C3" s="35"/>
+      <c r="D3" s="35"/>
+      <c r="E3" s="35"/>
+      <c r="F3" s="35"/>
+      <c r="G3" s="35"/>
+      <c r="H3" s="35"/>
     </row>
     <row r="4" spans="1:11" ht="26.4" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A4" s="4" t="s">
@@ -1451,14 +1451,14 @@
       </c>
     </row>
     <row r="5" spans="1:11" ht="32.4" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A5" s="28" t="s">
+      <c r="A5" s="27" t="s">
         <v>54</v>
       </c>
       <c r="B5" s="7" t="s">
         <v>51</v>
       </c>
       <c r="C5" s="7" t="s">
-        <v>53</v>
+        <v>27</v>
       </c>
       <c r="D5" s="7" t="s">
         <v>10</v>
@@ -1477,7 +1477,7 @@
       </c>
     </row>
     <row r="6" spans="1:11" ht="39.6" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A6" s="28" t="s">
+      <c r="A6" s="27" t="s">
         <v>0</v>
       </c>
       <c r="B6" s="7" t="s">
@@ -1504,7 +1504,7 @@
       <c r="I6" s="2"/>
     </row>
     <row r="7" spans="1:11" ht="52.2" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A7" s="29" t="s">
+      <c r="A7" s="28" t="s">
         <v>16</v>
       </c>
       <c r="B7" s="7" t="s">
@@ -1532,7 +1532,7 @@
       <c r="K7" s="2"/>
     </row>
     <row r="8" spans="1:11" ht="60" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A8" s="29" t="s">
+      <c r="A8" s="28" t="s">
         <v>40</v>
       </c>
       <c r="B8" s="7" t="s">
@@ -1557,7 +1557,7 @@
       <c r="J8" s="18"/>
     </row>
     <row r="9" spans="1:11" ht="59.4" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A9" s="30" t="s">
+      <c r="A9" s="29" t="s">
         <v>18</v>
       </c>
       <c r="B9" s="14" t="s">
@@ -1585,132 +1585,135 @@
       </c>
     </row>
     <row r="10" spans="1:11" ht="43.2" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A10" s="31" t="s">
+      <c r="A10" s="30" t="s">
         <v>39</v>
       </c>
-      <c r="B10" s="26" t="s">
+      <c r="B10" s="25" t="s">
         <v>9</v>
       </c>
-      <c r="C10" s="26" t="s">
+      <c r="C10" s="25" t="s">
         <v>2</v>
       </c>
-      <c r="D10" s="26" t="s">
+      <c r="D10" s="25" t="s">
         <v>10</v>
       </c>
-      <c r="E10" s="26">
+      <c r="E10" s="25">
         <v>1</v>
       </c>
-      <c r="F10" s="26">
+      <c r="F10" s="25">
         <v>2</v>
       </c>
-      <c r="G10" s="26">
+      <c r="G10" s="25">
         <v>6</v>
       </c>
-      <c r="H10" s="27"/>
+      <c r="H10" s="26"/>
       <c r="J10" s="13" t="s">
         <v>52</v>
       </c>
     </row>
     <row r="11" spans="1:11" ht="59.4" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A11" s="32" t="s">
+      <c r="A11" s="31" t="s">
         <v>14</v>
       </c>
-      <c r="B11" s="26" t="s">
+      <c r="B11" s="25" t="s">
         <v>15</v>
       </c>
-      <c r="C11" s="26" t="s">
+      <c r="C11" s="25" t="s">
         <v>12</v>
       </c>
-      <c r="D11" s="26" t="s">
+      <c r="D11" s="25" t="s">
         <v>60</v>
       </c>
-      <c r="E11" s="26">
+      <c r="E11" s="25">
         <v>1</v>
       </c>
-      <c r="F11" s="26">
+      <c r="F11" s="25">
         <v>2</v>
       </c>
-      <c r="G11" s="26">
+      <c r="G11" s="25">
         <v>6</v>
       </c>
-      <c r="H11" s="27"/>
+      <c r="H11" s="26"/>
     </row>
     <row r="12" spans="1:11" ht="39.6" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A12" s="31" t="s">
+      <c r="A12" s="32" t="s">
         <v>26</v>
       </c>
-      <c r="B12" s="26" t="s">
+      <c r="B12" s="11" t="s">
         <v>28</v>
       </c>
-      <c r="C12" s="26" t="s">
-        <v>27</v>
-      </c>
-      <c r="D12" s="26" t="s">
+      <c r="C12" s="11" t="s">
+        <v>53</v>
+      </c>
+      <c r="D12" s="11" t="s">
         <v>45</v>
       </c>
-      <c r="E12" s="26">
+      <c r="E12" s="11">
         <v>1</v>
       </c>
-      <c r="F12" s="26">
+      <c r="F12" s="11">
         <v>2</v>
       </c>
-      <c r="G12" s="26">
+      <c r="G12" s="11">
         <v>6</v>
       </c>
-      <c r="H12" s="27"/>
+      <c r="H12" s="23"/>
       <c r="I12" s="2"/>
+      <c r="J12" s="19" t="s">
+        <v>59</v>
+      </c>
     </row>
     <row r="13" spans="1:11" ht="47.4" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A13" s="31" t="s">
+      <c r="A13" s="30" t="s">
         <v>46</v>
       </c>
-      <c r="B13" s="26" t="s">
+      <c r="B13" s="25" t="s">
         <v>48</v>
       </c>
-      <c r="C13" s="26" t="s">
+      <c r="C13" s="25" t="s">
         <v>20</v>
       </c>
-      <c r="D13" s="26" t="s">
+      <c r="D13" s="25" t="s">
         <v>49</v>
       </c>
-      <c r="E13" s="26">
+      <c r="E13" s="25">
         <v>1</v>
       </c>
-      <c r="F13" s="26">
+      <c r="F13" s="25">
         <v>2</v>
       </c>
-      <c r="G13" s="26">
+      <c r="G13" s="25">
         <v>6</v>
       </c>
-      <c r="H13" s="27"/>
+      <c r="H13" s="26"/>
     </row>
     <row r="14" spans="1:11" ht="57.6" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A14" s="32" t="s">
+      <c r="A14" s="31" t="s">
         <v>47</v>
       </c>
-      <c r="B14" s="26" t="s">
+      <c r="B14" s="25" t="s">
         <v>50</v>
       </c>
-      <c r="C14" s="26" t="s">
+      <c r="C14" s="25" t="s">
         <v>20</v>
       </c>
-      <c r="D14" s="26" t="s">
+      <c r="D14" s="25" t="s">
         <v>10</v>
       </c>
-      <c r="E14" s="26">
+      <c r="E14" s="25">
         <v>1</v>
       </c>
-      <c r="F14" s="26">
+      <c r="F14" s="25">
         <v>2</v>
       </c>
-      <c r="G14" s="26">
+      <c r="G14" s="25">
         <v>6</v>
       </c>
-      <c r="H14" s="27"/>
+      <c r="H14" s="26"/>
       <c r="J14" s="20"/>
     </row>
     <row r="15" spans="1:11" ht="47.4" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A15" s="28" t="s">
+      <c r="A15" s="27" t="s">
         <v>29</v>
       </c>
       <c r="B15" s="7" t="s">
@@ -1734,7 +1737,7 @@
       <c r="H15" s="21"/>
     </row>
     <row r="16" spans="1:11" ht="57.6" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A16" s="33" t="s">
+      <c r="A16" s="32" t="s">
         <v>24</v>
       </c>
       <c r="B16" s="11" t="s">
@@ -1762,7 +1765,7 @@
       <c r="K16" s="2"/>
     </row>
     <row r="17" spans="1:10" ht="54.6" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A17" s="34" t="s">
+      <c r="A17" s="33" t="s">
         <v>21</v>
       </c>
       <c r="B17" s="11" t="s">
@@ -1790,7 +1793,7 @@
       </c>
     </row>
     <row r="18" spans="1:10" ht="48" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A18" s="29" t="s">
+      <c r="A18" s="28" t="s">
         <v>42</v>
       </c>
       <c r="B18" s="7" t="s">
@@ -1814,7 +1817,7 @@
       <c r="H18" s="21"/>
     </row>
     <row r="19" spans="1:10" ht="37.799999999999997" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A19" s="29" t="s">
+      <c r="A19" s="28" t="s">
         <v>34</v>
       </c>
       <c r="B19" s="7" t="s">
@@ -1838,7 +1841,7 @@
       <c r="H19" s="21"/>
     </row>
     <row r="20" spans="1:10" ht="39.6" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A20" s="29" t="s">
+      <c r="A20" s="28" t="s">
         <v>36</v>
       </c>
       <c r="B20" s="7" t="s">
@@ -1862,7 +1865,7 @@
       <c r="H20" s="21"/>
     </row>
     <row r="21" spans="1:10" ht="32.4" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A21" s="35" t="s">
+      <c r="A21" s="34" t="s">
         <v>37</v>
       </c>
       <c r="B21" s="9" t="s">

</xml_diff>

<commit_message>
ATCNS archived + study plan update
</commit_message>
<xml_diff>
--- a/MasterDegree_StudyPlan.xlsx
+++ b/MasterDegree_StudyPlan.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Michael\GitHub\Repo\Master-courses\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4BB20F9D-88D9-4B8A-B41B-F26557F59E0E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F3EA2B94-FC56-4F12-828F-F2ADAD7D9798}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{9CCEDFCE-005C-40C2-92E8-4E076261F21E}"/>
   </bookViews>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="79" uniqueCount="56">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="81" uniqueCount="57">
   <si>
     <t>Computability</t>
   </si>
@@ -228,6 +228,9 @@
   </si>
   <si>
     <t>CHOOSE A COURSE</t>
+  </si>
+  <si>
+    <t>Law and data?</t>
   </si>
 </sst>
 </file>
@@ -472,7 +475,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="35">
+  <cellXfs count="39">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -503,9 +506,6 @@
     <xf numFmtId="0" fontId="1" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
@@ -570,6 +570,21 @@
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="4" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
@@ -1363,7 +1378,7 @@
   <dimension ref="A1:K22"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="J2" sqref="J2"/>
+      <selection activeCell="J14" sqref="J14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1382,36 +1397,36 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:11" x14ac:dyDescent="0.3">
-      <c r="A1" s="34" t="s">
+      <c r="A1" s="33" t="s">
         <v>37</v>
       </c>
-      <c r="B1" s="34"/>
-      <c r="C1" s="34"/>
-      <c r="D1" s="34"/>
-      <c r="E1" s="34"/>
-      <c r="F1" s="34"/>
-      <c r="G1" s="34"/>
-      <c r="H1" s="34"/>
+      <c r="B1" s="33"/>
+      <c r="C1" s="33"/>
+      <c r="D1" s="33"/>
+      <c r="E1" s="33"/>
+      <c r="F1" s="33"/>
+      <c r="G1" s="33"/>
+      <c r="H1" s="33"/>
     </row>
     <row r="2" spans="1:11" x14ac:dyDescent="0.3">
-      <c r="A2" s="34"/>
-      <c r="B2" s="34"/>
-      <c r="C2" s="34"/>
-      <c r="D2" s="34"/>
-      <c r="E2" s="34"/>
-      <c r="F2" s="34"/>
-      <c r="G2" s="34"/>
-      <c r="H2" s="34"/>
+      <c r="A2" s="33"/>
+      <c r="B2" s="33"/>
+      <c r="C2" s="33"/>
+      <c r="D2" s="33"/>
+      <c r="E2" s="33"/>
+      <c r="F2" s="33"/>
+      <c r="G2" s="33"/>
+      <c r="H2" s="33"/>
     </row>
     <row r="3" spans="1:11" x14ac:dyDescent="0.3">
-      <c r="A3" s="34"/>
-      <c r="B3" s="34"/>
-      <c r="C3" s="34"/>
-      <c r="D3" s="34"/>
-      <c r="E3" s="34"/>
-      <c r="F3" s="34"/>
-      <c r="G3" s="34"/>
-      <c r="H3" s="34"/>
+      <c r="A3" s="33"/>
+      <c r="B3" s="33"/>
+      <c r="C3" s="33"/>
+      <c r="D3" s="33"/>
+      <c r="E3" s="33"/>
+      <c r="F3" s="33"/>
+      <c r="G3" s="33"/>
+      <c r="H3" s="33"/>
     </row>
     <row r="4" spans="1:11" ht="33.6" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A4" s="4" t="s">
@@ -1438,12 +1453,12 @@
       <c r="H4" s="6" t="s">
         <v>51</v>
       </c>
-      <c r="J4" s="29" t="s">
+      <c r="J4" s="28" t="s">
         <v>53</v>
       </c>
     </row>
     <row r="5" spans="1:11" ht="32.4" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A5" s="20" t="s">
+      <c r="A5" s="19" t="s">
         <v>48</v>
       </c>
       <c r="B5" s="7" t="s">
@@ -1464,15 +1479,15 @@
       <c r="G5" s="7">
         <v>6</v>
       </c>
-      <c r="H5" s="14" t="s">
+      <c r="H5" s="13" t="s">
         <v>31</v>
       </c>
-      <c r="J5" s="30" t="s">
+      <c r="J5" s="29" t="s">
         <v>46</v>
       </c>
     </row>
     <row r="6" spans="1:11" ht="39.6" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A6" s="20" t="s">
+      <c r="A6" s="19" t="s">
         <v>0</v>
       </c>
       <c r="B6" s="7" t="s">
@@ -1493,16 +1508,16 @@
       <c r="G6" s="7">
         <v>6</v>
       </c>
-      <c r="H6" s="14" t="s">
+      <c r="H6" s="13" t="s">
         <v>31</v>
       </c>
       <c r="I6" s="2"/>
-      <c r="J6" s="31" t="s">
+      <c r="J6" s="30" t="s">
         <v>50</v>
       </c>
     </row>
     <row r="7" spans="1:11" ht="52.2" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A7" s="21" t="s">
+      <c r="A7" s="20" t="s">
         <v>16</v>
       </c>
       <c r="B7" s="7" t="s">
@@ -1523,16 +1538,16 @@
       <c r="G7" s="7">
         <v>6</v>
       </c>
-      <c r="H7" s="14" t="s">
+      <c r="H7" s="13" t="s">
         <v>31</v>
       </c>
-      <c r="J7" s="32" t="s">
+      <c r="J7" s="31" t="s">
         <v>55</v>
       </c>
-      <c r="K7" s="27"/>
+      <c r="K7" s="26"/>
     </row>
     <row r="8" spans="1:11" ht="53.4" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A8" s="21" t="s">
+      <c r="A8" s="20" t="s">
         <v>36</v>
       </c>
       <c r="B8" s="7" t="s">
@@ -1541,24 +1556,24 @@
       <c r="C8" s="7" t="s">
         <v>2</v>
       </c>
-      <c r="D8" s="33" t="s">
+      <c r="D8" s="32" t="s">
         <v>10</v>
       </c>
       <c r="E8" s="7">
         <v>1</v>
       </c>
       <c r="F8" s="7">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="G8" s="7">
         <v>6</v>
       </c>
-      <c r="H8" s="14" t="s">
+      <c r="H8" s="13" t="s">
         <v>31</v>
       </c>
     </row>
     <row r="9" spans="1:11" ht="59.4" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A9" s="20" t="s">
+      <c r="A9" s="19" t="s">
         <v>35</v>
       </c>
       <c r="B9" s="7" t="s">
@@ -1579,111 +1594,115 @@
       <c r="G9" s="7">
         <v>6</v>
       </c>
-      <c r="H9" s="14" t="s">
+      <c r="H9" s="13" t="s">
         <v>31</v>
       </c>
       <c r="I9" s="2"/>
     </row>
-    <row r="10" spans="1:11" ht="49.2" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A10" s="22" t="s">
+    <row r="10" spans="1:11" ht="55.2" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A10" s="34" t="s">
+        <v>18</v>
+      </c>
+      <c r="B10" s="35" t="s">
+        <v>19</v>
+      </c>
+      <c r="C10" s="35" t="s">
+        <v>12</v>
+      </c>
+      <c r="D10" s="36" t="s">
+        <v>49</v>
+      </c>
+      <c r="E10" s="35">
+        <v>1</v>
+      </c>
+      <c r="F10" s="35">
+        <v>2</v>
+      </c>
+      <c r="G10" s="35">
+        <v>6</v>
+      </c>
+      <c r="H10" s="37" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="11" spans="1:11" ht="52.2" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A11" s="21" t="s">
         <v>14</v>
       </c>
-      <c r="B10" s="11" t="s">
+      <c r="B11" s="11" t="s">
         <v>15</v>
       </c>
-      <c r="C10" s="11" t="s">
+      <c r="C11" s="11" t="s">
         <v>12</v>
       </c>
-      <c r="D10" s="11" t="s">
+      <c r="D11" s="11" t="s">
         <v>52</v>
       </c>
-      <c r="E10" s="11">
+      <c r="E11" s="11">
         <v>1</v>
       </c>
-      <c r="F10" s="11">
+      <c r="F11" s="11">
         <v>2</v>
       </c>
-      <c r="G10" s="11">
+      <c r="G11" s="11">
         <v>6</v>
       </c>
-      <c r="H10" s="15"/>
-    </row>
-    <row r="11" spans="1:11" ht="52.2" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A11" s="23" t="s">
+      <c r="H11" s="14"/>
+    </row>
+    <row r="12" spans="1:11" ht="64.8" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A12" s="38" t="s">
         <v>42</v>
       </c>
-      <c r="B11" s="18" t="s">
+      <c r="B12" s="11" t="s">
         <v>43</v>
       </c>
-      <c r="C11" s="18" t="s">
+      <c r="C12" s="11" t="s">
         <v>20</v>
       </c>
-      <c r="D11" s="18" t="s">
+      <c r="D12" s="11" t="s">
         <v>44</v>
       </c>
-      <c r="E11" s="18">
+      <c r="E12" s="11">
         <v>1</v>
       </c>
-      <c r="F11" s="18">
+      <c r="F12" s="11">
         <v>2</v>
       </c>
-      <c r="G11" s="18">
+      <c r="G12" s="11">
         <v>6</v>
       </c>
-      <c r="H11" s="19"/>
-    </row>
-    <row r="12" spans="1:11" ht="64.8" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A12" s="23" t="s">
-        <v>24</v>
-      </c>
-      <c r="B12" s="18" t="s">
-        <v>25</v>
-      </c>
-      <c r="C12" s="18" t="s">
-        <v>20</v>
-      </c>
-      <c r="D12" s="28" t="s">
-        <v>40</v>
-      </c>
-      <c r="E12" s="18">
-        <v>1</v>
-      </c>
-      <c r="F12" s="18">
-        <v>2</v>
-      </c>
-      <c r="G12" s="18">
-        <v>6</v>
-      </c>
-      <c r="H12" s="19"/>
+      <c r="H12" s="14"/>
       <c r="I12" s="2"/>
     </row>
     <row r="13" spans="1:11" ht="61.8" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A13" s="22" t="s">
-        <v>18</v>
-      </c>
-      <c r="B13" s="11" t="s">
-        <v>19</v>
-      </c>
-      <c r="C13" s="11" t="s">
-        <v>12</v>
-      </c>
-      <c r="D13" s="12" t="s">
-        <v>49</v>
-      </c>
-      <c r="E13" s="11">
+        <v>24</v>
+      </c>
+      <c r="B13" s="17" t="s">
+        <v>25</v>
+      </c>
+      <c r="C13" s="17" t="s">
+        <v>20</v>
+      </c>
+      <c r="D13" s="27" t="s">
+        <v>40</v>
+      </c>
+      <c r="E13" s="17">
         <v>1</v>
       </c>
-      <c r="F13" s="11">
-        <v>1</v>
-      </c>
-      <c r="G13" s="11">
+      <c r="F13" s="17">
+        <v>2</v>
+      </c>
+      <c r="G13" s="17">
         <v>6</v>
       </c>
-      <c r="H13" s="15"/>
-      <c r="J13" s="27"/>
+      <c r="H13" s="18"/>
+      <c r="J13" s="26"/>
     </row>
     <row r="14" spans="1:11" ht="66.599999999999994" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A14" s="25"/>
+      <c r="A14" s="24" t="s">
+        <v>56</v>
+      </c>
       <c r="B14" s="10"/>
       <c r="C14" s="10" t="s">
         <v>47</v>
@@ -1698,11 +1717,11 @@
       <c r="G14" s="10">
         <v>6</v>
       </c>
-      <c r="H14" s="16"/>
-      <c r="J14" s="13"/>
+      <c r="H14" s="15"/>
+      <c r="J14" s="12"/>
     </row>
     <row r="15" spans="1:11" ht="47.4" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A15" s="24"/>
+      <c r="A15" s="23"/>
       <c r="B15" s="10"/>
       <c r="C15" s="10" t="s">
         <v>47</v>
@@ -1717,10 +1736,10 @@
       <c r="G15" s="10">
         <v>6</v>
       </c>
-      <c r="H15" s="16"/>
+      <c r="H15" s="15"/>
     </row>
     <row r="16" spans="1:11" ht="57.6" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A16" s="21" t="s">
+      <c r="A16" s="20" t="s">
         <v>21</v>
       </c>
       <c r="B16" s="7" t="s">
@@ -1729,7 +1748,7 @@
       <c r="C16" s="7" t="s">
         <v>20</v>
       </c>
-      <c r="D16" s="33" t="s">
+      <c r="D16" s="32" t="s">
         <v>23</v>
       </c>
       <c r="E16" s="7">
@@ -1741,12 +1760,12 @@
       <c r="G16" s="7">
         <v>6</v>
       </c>
-      <c r="H16" s="14"/>
-      <c r="J16" s="27"/>
+      <c r="H16" s="13"/>
+      <c r="J16" s="26"/>
       <c r="K16" s="2"/>
     </row>
     <row r="17" spans="1:9" ht="54.6" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A17" s="20" t="s">
+      <c r="A17" s="19" t="s">
         <v>27</v>
       </c>
       <c r="B17" s="7" t="s">
@@ -1767,11 +1786,11 @@
       <c r="G17" s="7">
         <v>3</v>
       </c>
-      <c r="H17" s="14"/>
+      <c r="H17" s="13"/>
       <c r="I17" s="9"/>
     </row>
     <row r="18" spans="1:9" ht="48" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A18" s="21" t="s">
+      <c r="A18" s="20" t="s">
         <v>38</v>
       </c>
       <c r="B18" s="7" t="s">
@@ -1792,10 +1811,10 @@
       <c r="G18" s="7">
         <v>6</v>
       </c>
-      <c r="H18" s="14"/>
+      <c r="H18" s="13"/>
     </row>
     <row r="19" spans="1:9" ht="37.799999999999997" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A19" s="21" t="s">
+      <c r="A19" s="20" t="s">
         <v>54</v>
       </c>
       <c r="B19" s="7" t="s">
@@ -1816,10 +1835,10 @@
       <c r="G19" s="7">
         <v>6</v>
       </c>
-      <c r="H19" s="14"/>
+      <c r="H19" s="13"/>
     </row>
     <row r="20" spans="1:9" ht="39.6" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A20" s="26" t="s">
+      <c r="A20" s="25" t="s">
         <v>33</v>
       </c>
       <c r="B20" s="8" t="s">
@@ -1840,7 +1859,7 @@
       <c r="G20" s="8">
         <v>33</v>
       </c>
-      <c r="H20" s="17"/>
+      <c r="H20" s="16"/>
     </row>
     <row r="21" spans="1:9" ht="32.4" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A21" s="1"/>

</xml_diff>

<commit_message>
repo updated after today MPM exam
</commit_message>
<xml_diff>
--- a/MasterDegree_StudyPlan.xlsx
+++ b/MasterDegree_StudyPlan.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Michael\GitHub\Repo\Master-courses\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B7ADC5C4-7EDA-4A70-84C2-BE7370A38012}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E8910442-0B13-4A74-AA16-37260909C6BB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{9CCEDFCE-005C-40C2-92E8-4E076261F21E}"/>
   </bookViews>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="88" uniqueCount="60">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="89" uniqueCount="60">
   <si>
     <t>Computability</t>
   </si>
@@ -212,9 +212,6 @@
     <t>Team project + written</t>
   </si>
   <si>
-    <t>Report during the course + multiple choice final test</t>
-  </si>
-  <si>
     <t>Start-Up in ICT</t>
   </si>
   <si>
@@ -240,6 +237,9 @@
   </si>
   <si>
     <t>2/ 6 credits awarded</t>
+  </si>
+  <si>
+    <t>Two reports during the course + multiple choice final test</t>
   </si>
 </sst>
 </file>
@@ -478,7 +478,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="32">
+  <cellXfs count="31">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -524,9 +524,6 @@
     <xf numFmtId="0" fontId="8" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="8" fillId="3" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="8" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -548,6 +545,12 @@
     <xf numFmtId="0" fontId="1" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -560,14 +563,8 @@
     <xf numFmtId="0" fontId="8" fillId="0" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="3" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    <xf numFmtId="0" fontId="11" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -1359,8 +1356,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{89E4B725-BD0D-4291-9550-3225AF05D5FC}">
   <dimension ref="A1:K22"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A10" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="J13" sqref="J13"/>
+    <sheetView tabSelected="1" topLeftCell="A8" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="J12" sqref="J12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1379,36 +1376,36 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:11" x14ac:dyDescent="0.3">
-      <c r="A1" s="25" t="s">
+      <c r="A1" s="26" t="s">
         <v>34</v>
       </c>
-      <c r="B1" s="25"/>
-      <c r="C1" s="25"/>
-      <c r="D1" s="25"/>
-      <c r="E1" s="25"/>
-      <c r="F1" s="25"/>
-      <c r="G1" s="25"/>
-      <c r="H1" s="25"/>
+      <c r="B1" s="26"/>
+      <c r="C1" s="26"/>
+      <c r="D1" s="26"/>
+      <c r="E1" s="26"/>
+      <c r="F1" s="26"/>
+      <c r="G1" s="26"/>
+      <c r="H1" s="26"/>
     </row>
     <row r="2" spans="1:11" x14ac:dyDescent="0.3">
-      <c r="A2" s="25"/>
-      <c r="B2" s="25"/>
-      <c r="C2" s="25"/>
-      <c r="D2" s="25"/>
-      <c r="E2" s="25"/>
-      <c r="F2" s="25"/>
-      <c r="G2" s="25"/>
-      <c r="H2" s="25"/>
+      <c r="A2" s="26"/>
+      <c r="B2" s="26"/>
+      <c r="C2" s="26"/>
+      <c r="D2" s="26"/>
+      <c r="E2" s="26"/>
+      <c r="F2" s="26"/>
+      <c r="G2" s="26"/>
+      <c r="H2" s="26"/>
     </row>
     <row r="3" spans="1:11" x14ac:dyDescent="0.3">
-      <c r="A3" s="25"/>
-      <c r="B3" s="25"/>
-      <c r="C3" s="25"/>
-      <c r="D3" s="25"/>
-      <c r="E3" s="25"/>
-      <c r="F3" s="25"/>
-      <c r="G3" s="25"/>
-      <c r="H3" s="25"/>
+      <c r="A3" s="26"/>
+      <c r="B3" s="26"/>
+      <c r="C3" s="26"/>
+      <c r="D3" s="26"/>
+      <c r="E3" s="26"/>
+      <c r="F3" s="26"/>
+      <c r="G3" s="26"/>
+      <c r="H3" s="26"/>
     </row>
     <row r="4" spans="1:11" ht="33.6" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A4" s="4" t="s">
@@ -1435,7 +1432,7 @@
       <c r="H4" s="6" t="s">
         <v>45</v>
       </c>
-      <c r="J4" s="20" t="s">
+      <c r="J4" s="19" t="s">
         <v>47</v>
       </c>
     </row>
@@ -1464,7 +1461,7 @@
       <c r="H5" s="12" t="s">
         <v>29</v>
       </c>
-      <c r="J5" s="21" t="s">
+      <c r="J5" s="20" t="s">
         <v>41</v>
       </c>
     </row>
@@ -1523,8 +1520,8 @@
       <c r="H7" s="12" t="s">
         <v>29</v>
       </c>
-      <c r="J7" s="31"/>
-      <c r="K7" s="19"/>
+      <c r="J7" s="25"/>
+      <c r="K7" s="18"/>
     </row>
     <row r="8" spans="1:11" ht="61.8" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A8" s="16" t="s">
@@ -1536,7 +1533,7 @@
       <c r="C8" s="7" t="s">
         <v>2</v>
       </c>
-      <c r="D8" s="22" t="s">
+      <c r="D8" s="21" t="s">
         <v>10</v>
       </c>
       <c r="E8" s="7">
@@ -1589,7 +1586,7 @@
       <c r="C10" s="7" t="s">
         <v>12</v>
       </c>
-      <c r="D10" s="22" t="s">
+      <c r="D10" s="21" t="s">
         <v>43</v>
       </c>
       <c r="E10" s="7">
@@ -1607,7 +1604,7 @@
     </row>
     <row r="11" spans="1:11" ht="52.2" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A11" s="15" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="B11" s="7" t="s">
         <v>39</v>
@@ -1632,32 +1629,34 @@
       </c>
     </row>
     <row r="12" spans="1:11" ht="64.8" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A12" s="17" t="s">
+      <c r="A12" s="27" t="s">
         <v>13</v>
       </c>
-      <c r="B12" s="10" t="s">
+      <c r="B12" s="28" t="s">
         <v>14</v>
       </c>
-      <c r="C12" s="10" t="s">
+      <c r="C12" s="28" t="s">
         <v>12</v>
       </c>
-      <c r="D12" s="10" t="s">
+      <c r="D12" s="28" t="s">
         <v>46</v>
       </c>
-      <c r="E12" s="10">
+      <c r="E12" s="28">
         <v>1</v>
       </c>
-      <c r="F12" s="10">
+      <c r="F12" s="28">
         <v>2</v>
       </c>
-      <c r="G12" s="10">
+      <c r="G12" s="28">
         <v>6</v>
       </c>
-      <c r="H12" s="13"/>
+      <c r="H12" s="29" t="s">
+        <v>29</v>
+      </c>
       <c r="I12" s="2"/>
     </row>
     <row r="13" spans="1:11" ht="61.8" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A13" s="23" t="s">
+      <c r="A13" s="22" t="s">
         <v>22</v>
       </c>
       <c r="B13" s="10" t="s">
@@ -1666,7 +1665,7 @@
       <c r="C13" s="10" t="s">
         <v>19</v>
       </c>
-      <c r="D13" s="24" t="s">
+      <c r="D13" s="23" t="s">
         <v>37</v>
       </c>
       <c r="E13" s="10">
@@ -1679,7 +1678,7 @@
         <v>6</v>
       </c>
       <c r="H13" s="13"/>
-      <c r="J13" s="19"/>
+      <c r="J13" s="18"/>
     </row>
     <row r="14" spans="1:11" ht="61.8" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A14" s="16" t="s">
@@ -1704,7 +1703,7 @@
         <v>6</v>
       </c>
       <c r="H14" s="12"/>
-      <c r="J14" s="19"/>
+      <c r="J14" s="18"/>
     </row>
     <row r="15" spans="1:11" ht="61.8" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A15" s="16" t="s">
@@ -1716,8 +1715,8 @@
       <c r="C15" s="7" t="s">
         <v>19</v>
       </c>
-      <c r="D15" s="22" t="s">
-        <v>50</v>
+      <c r="D15" s="21" t="s">
+        <v>59</v>
       </c>
       <c r="E15" s="7">
         <v>2</v>
@@ -1729,56 +1728,56 @@
         <v>6</v>
       </c>
       <c r="H15" s="12"/>
-      <c r="J15" s="19"/>
+      <c r="J15" s="18"/>
     </row>
     <row r="16" spans="1:11" ht="66.599999999999994" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A16" s="26" t="s">
+      <c r="A16" s="16" t="s">
+        <v>51</v>
+      </c>
+      <c r="B16" s="7" t="s">
+        <v>53</v>
+      </c>
+      <c r="C16" s="7" t="s">
+        <v>57</v>
+      </c>
+      <c r="D16" s="7" t="s">
+        <v>10</v>
+      </c>
+      <c r="E16" s="7">
+        <v>2</v>
+      </c>
+      <c r="F16" s="7">
+        <v>1</v>
+      </c>
+      <c r="G16" s="7">
+        <v>6</v>
+      </c>
+      <c r="H16" s="12"/>
+      <c r="J16" s="11"/>
+    </row>
+    <row r="17" spans="1:10" ht="58.8" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A17" s="16" t="s">
         <v>52</v>
       </c>
-      <c r="B16" s="27" t="s">
+      <c r="B17" s="7" t="s">
         <v>54</v>
       </c>
-      <c r="C16" s="27" t="s">
-        <v>58</v>
-      </c>
-      <c r="D16" s="27" t="s">
+      <c r="C17" s="7" t="s">
+        <v>57</v>
+      </c>
+      <c r="D17" s="7" t="s">
         <v>10</v>
       </c>
-      <c r="E16" s="27">
+      <c r="E17" s="7">
         <v>2</v>
       </c>
-      <c r="F16" s="27">
+      <c r="F17" s="7">
         <v>1</v>
       </c>
-      <c r="G16" s="27">
+      <c r="G17" s="7">
         <v>6</v>
       </c>
-      <c r="H16" s="28"/>
-      <c r="J16" s="11"/>
-    </row>
-    <row r="17" spans="1:10" ht="58.8" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A17" s="26" t="s">
-        <v>53</v>
-      </c>
-      <c r="B17" s="27" t="s">
-        <v>55</v>
-      </c>
-      <c r="C17" s="27" t="s">
-        <v>58</v>
-      </c>
-      <c r="D17" s="27" t="s">
-        <v>10</v>
-      </c>
-      <c r="E17" s="27">
-        <v>2</v>
-      </c>
-      <c r="F17" s="27">
-        <v>1</v>
-      </c>
-      <c r="G17" s="27">
-        <v>6</v>
-      </c>
-      <c r="H17" s="28"/>
+      <c r="H17" s="12"/>
     </row>
     <row r="18" spans="1:10" ht="54.6" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A18" s="15" t="s">
@@ -1791,7 +1790,7 @@
         <v>2</v>
       </c>
       <c r="D18" s="7" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="E18" s="7">
         <v>2</v>
@@ -1809,8 +1808,8 @@
       <c r="A19" s="16" t="s">
         <v>48</v>
       </c>
-      <c r="B19" s="22" t="s">
-        <v>56</v>
+      <c r="B19" s="21" t="s">
+        <v>55</v>
       </c>
       <c r="C19" s="7" t="s">
         <v>2</v>
@@ -1828,12 +1827,12 @@
         <v>6</v>
       </c>
       <c r="H19" s="12"/>
-      <c r="J19" s="29" t="s">
-        <v>59</v>
+      <c r="J19" s="24" t="s">
+        <v>58</v>
       </c>
     </row>
     <row r="20" spans="1:10" ht="39.6" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A20" s="18" t="s">
+      <c r="A20" s="17" t="s">
         <v>31</v>
       </c>
       <c r="B20" s="8" t="s">

</xml_diff>

<commit_message>
general update after today ITSM exam
</commit_message>
<xml_diff>
--- a/MasterDegree_StudyPlan.xlsx
+++ b/MasterDegree_StudyPlan.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Michael\GitHub\Repo\Master-courses\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E8910442-0B13-4A74-AA16-37260909C6BB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{65DBC2C5-FEEA-433E-A6DC-D39F7F87D68A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{9CCEDFCE-005C-40C2-92E8-4E076261F21E}"/>
   </bookViews>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="89" uniqueCount="60">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="90" uniqueCount="60">
   <si>
     <t>Computability</t>
   </si>
@@ -478,7 +478,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="31">
+  <cellXfs count="32">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -503,18 +503,12 @@
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="1" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
     <xf numFmtId="0" fontId="8" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="8" fillId="3" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="8" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -539,32 +533,41 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="8" fillId="3" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="11" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="11" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="8" fillId="0" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="8" fillId="0" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="11" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
+    <xf numFmtId="0" fontId="8" fillId="2" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="2" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -1356,8 +1359,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{89E4B725-BD0D-4291-9550-3225AF05D5FC}">
   <dimension ref="A1:K22"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A8" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="J12" sqref="J12"/>
+    <sheetView tabSelected="1" topLeftCell="A12" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="J18" sqref="J18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1376,36 +1379,36 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:11" x14ac:dyDescent="0.3">
-      <c r="A1" s="26" t="s">
+      <c r="A1" s="23" t="s">
         <v>34</v>
       </c>
-      <c r="B1" s="26"/>
-      <c r="C1" s="26"/>
-      <c r="D1" s="26"/>
-      <c r="E1" s="26"/>
-      <c r="F1" s="26"/>
-      <c r="G1" s="26"/>
-      <c r="H1" s="26"/>
+      <c r="B1" s="23"/>
+      <c r="C1" s="23"/>
+      <c r="D1" s="23"/>
+      <c r="E1" s="23"/>
+      <c r="F1" s="23"/>
+      <c r="G1" s="23"/>
+      <c r="H1" s="23"/>
     </row>
     <row r="2" spans="1:11" x14ac:dyDescent="0.3">
-      <c r="A2" s="26"/>
-      <c r="B2" s="26"/>
-      <c r="C2" s="26"/>
-      <c r="D2" s="26"/>
-      <c r="E2" s="26"/>
-      <c r="F2" s="26"/>
-      <c r="G2" s="26"/>
-      <c r="H2" s="26"/>
+      <c r="A2" s="23"/>
+      <c r="B2" s="23"/>
+      <c r="C2" s="23"/>
+      <c r="D2" s="23"/>
+      <c r="E2" s="23"/>
+      <c r="F2" s="23"/>
+      <c r="G2" s="23"/>
+      <c r="H2" s="23"/>
     </row>
     <row r="3" spans="1:11" x14ac:dyDescent="0.3">
-      <c r="A3" s="26"/>
-      <c r="B3" s="26"/>
-      <c r="C3" s="26"/>
-      <c r="D3" s="26"/>
-      <c r="E3" s="26"/>
-      <c r="F3" s="26"/>
-      <c r="G3" s="26"/>
-      <c r="H3" s="26"/>
+      <c r="A3" s="23"/>
+      <c r="B3" s="23"/>
+      <c r="C3" s="23"/>
+      <c r="D3" s="23"/>
+      <c r="E3" s="23"/>
+      <c r="F3" s="23"/>
+      <c r="G3" s="23"/>
+      <c r="H3" s="23"/>
     </row>
     <row r="4" spans="1:11" ht="33.6" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A4" s="4" t="s">
@@ -1432,12 +1435,12 @@
       <c r="H4" s="6" t="s">
         <v>45</v>
       </c>
-      <c r="J4" s="19" t="s">
+      <c r="J4" s="17" t="s">
         <v>47</v>
       </c>
     </row>
-    <row r="5" spans="1:11" ht="32.4" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A5" s="15" t="s">
+    <row r="5" spans="1:11" ht="42.6" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A5" s="13" t="s">
         <v>42</v>
       </c>
       <c r="B5" s="7" t="s">
@@ -1458,15 +1461,15 @@
       <c r="G5" s="7">
         <v>6</v>
       </c>
-      <c r="H5" s="12" t="s">
+      <c r="H5" s="11" t="s">
         <v>29</v>
       </c>
-      <c r="J5" s="20" t="s">
+      <c r="J5" s="18" t="s">
         <v>41</v>
       </c>
     </row>
     <row r="6" spans="1:11" ht="39.6" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A6" s="15" t="s">
+      <c r="A6" s="13" t="s">
         <v>0</v>
       </c>
       <c r="B6" s="7" t="s">
@@ -1487,16 +1490,16 @@
       <c r="G6" s="7">
         <v>6</v>
       </c>
-      <c r="H6" s="12" t="s">
+      <c r="H6" s="11" t="s">
         <v>29</v>
       </c>
       <c r="I6" s="2"/>
-      <c r="J6" s="30" t="s">
+      <c r="J6" s="22" t="s">
         <v>44</v>
       </c>
     </row>
     <row r="7" spans="1:11" ht="52.2" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A7" s="16" t="s">
+      <c r="A7" s="14" t="s">
         <v>15</v>
       </c>
       <c r="B7" s="7" t="s">
@@ -1517,14 +1520,14 @@
       <c r="G7" s="7">
         <v>6</v>
       </c>
-      <c r="H7" s="12" t="s">
+      <c r="H7" s="11" t="s">
         <v>29</v>
       </c>
-      <c r="J7" s="25"/>
-      <c r="K7" s="18"/>
+      <c r="J7" s="21"/>
+      <c r="K7" s="16"/>
     </row>
     <row r="8" spans="1:11" ht="61.8" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A8" s="16" t="s">
+      <c r="A8" s="14" t="s">
         <v>33</v>
       </c>
       <c r="B8" s="7" t="s">
@@ -1533,7 +1536,7 @@
       <c r="C8" s="7" t="s">
         <v>2</v>
       </c>
-      <c r="D8" s="21" t="s">
+      <c r="D8" s="19" t="s">
         <v>10</v>
       </c>
       <c r="E8" s="7">
@@ -1545,12 +1548,12 @@
       <c r="G8" s="7">
         <v>6</v>
       </c>
-      <c r="H8" s="12" t="s">
+      <c r="H8" s="11" t="s">
         <v>29</v>
       </c>
     </row>
     <row r="9" spans="1:11" ht="59.4" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A9" s="15" t="s">
+      <c r="A9" s="13" t="s">
         <v>32</v>
       </c>
       <c r="B9" s="7" t="s">
@@ -1571,13 +1574,13 @@
       <c r="G9" s="7">
         <v>6</v>
       </c>
-      <c r="H9" s="12" t="s">
+      <c r="H9" s="11" t="s">
         <v>29</v>
       </c>
       <c r="I9" s="2"/>
     </row>
     <row r="10" spans="1:11" ht="72.599999999999994" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A10" s="16" t="s">
+      <c r="A10" s="14" t="s">
         <v>17</v>
       </c>
       <c r="B10" s="7" t="s">
@@ -1586,7 +1589,7 @@
       <c r="C10" s="7" t="s">
         <v>12</v>
       </c>
-      <c r="D10" s="21" t="s">
+      <c r="D10" s="19" t="s">
         <v>43</v>
       </c>
       <c r="E10" s="7">
@@ -1598,12 +1601,12 @@
       <c r="G10" s="7">
         <v>6</v>
       </c>
-      <c r="H10" s="12" t="s">
+      <c r="H10" s="11" t="s">
         <v>29</v>
       </c>
     </row>
     <row r="11" spans="1:11" ht="52.2" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A11" s="15" t="s">
+      <c r="A11" s="13" t="s">
         <v>50</v>
       </c>
       <c r="B11" s="7" t="s">
@@ -1624,163 +1627,165 @@
       <c r="G11" s="7">
         <v>6</v>
       </c>
-      <c r="H11" s="12" t="s">
+      <c r="H11" s="11" t="s">
         <v>29</v>
       </c>
     </row>
     <row r="12" spans="1:11" ht="64.8" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A12" s="27" t="s">
+      <c r="A12" s="14" t="s">
         <v>13</v>
       </c>
-      <c r="B12" s="28" t="s">
+      <c r="B12" s="7" t="s">
         <v>14</v>
       </c>
-      <c r="C12" s="28" t="s">
+      <c r="C12" s="7" t="s">
         <v>12</v>
       </c>
-      <c r="D12" s="28" t="s">
+      <c r="D12" s="7" t="s">
         <v>46</v>
       </c>
-      <c r="E12" s="28">
+      <c r="E12" s="7">
         <v>1</v>
       </c>
-      <c r="F12" s="28">
+      <c r="F12" s="7">
         <v>2</v>
       </c>
-      <c r="G12" s="28">
+      <c r="G12" s="7">
         <v>6</v>
       </c>
-      <c r="H12" s="29" t="s">
+      <c r="H12" s="11" t="s">
         <v>29</v>
       </c>
       <c r="I12" s="2"/>
     </row>
     <row r="13" spans="1:11" ht="61.8" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A13" s="22" t="s">
+      <c r="A13" s="24" t="s">
         <v>22</v>
       </c>
-      <c r="B13" s="10" t="s">
+      <c r="B13" s="25" t="s">
         <v>23</v>
       </c>
-      <c r="C13" s="10" t="s">
+      <c r="C13" s="25" t="s">
         <v>19</v>
       </c>
-      <c r="D13" s="23" t="s">
+      <c r="D13" s="26" t="s">
         <v>37</v>
       </c>
-      <c r="E13" s="10">
+      <c r="E13" s="25">
         <v>1</v>
       </c>
-      <c r="F13" s="10">
+      <c r="F13" s="25">
         <v>2</v>
       </c>
-      <c r="G13" s="10">
+      <c r="G13" s="25">
         <v>6</v>
       </c>
-      <c r="H13" s="13"/>
-      <c r="J13" s="18"/>
+      <c r="H13" s="27" t="s">
+        <v>29</v>
+      </c>
+      <c r="J13" s="16"/>
     </row>
     <row r="14" spans="1:11" ht="61.8" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A14" s="16" t="s">
+      <c r="A14" s="28" t="s">
         <v>35</v>
       </c>
-      <c r="B14" s="7" t="s">
+      <c r="B14" s="29" t="s">
         <v>11</v>
       </c>
-      <c r="C14" s="7" t="s">
+      <c r="C14" s="29" t="s">
         <v>12</v>
       </c>
-      <c r="D14" s="7" t="s">
+      <c r="D14" s="29" t="s">
         <v>36</v>
       </c>
-      <c r="E14" s="7">
+      <c r="E14" s="29">
         <v>2</v>
       </c>
-      <c r="F14" s="7">
+      <c r="F14" s="29">
         <v>1</v>
       </c>
-      <c r="G14" s="7">
+      <c r="G14" s="29">
         <v>6</v>
       </c>
-      <c r="H14" s="12"/>
-      <c r="J14" s="18"/>
+      <c r="H14" s="30"/>
+      <c r="J14" s="16"/>
     </row>
     <row r="15" spans="1:11" ht="61.8" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A15" s="16" t="s">
+      <c r="A15" s="28" t="s">
         <v>20</v>
       </c>
-      <c r="B15" s="7" t="s">
+      <c r="B15" s="29" t="s">
         <v>21</v>
       </c>
-      <c r="C15" s="7" t="s">
+      <c r="C15" s="29" t="s">
         <v>19</v>
       </c>
-      <c r="D15" s="21" t="s">
+      <c r="D15" s="31" t="s">
         <v>59</v>
       </c>
-      <c r="E15" s="7">
+      <c r="E15" s="29">
         <v>2</v>
       </c>
-      <c r="F15" s="7">
+      <c r="F15" s="29">
         <v>1</v>
       </c>
-      <c r="G15" s="7">
+      <c r="G15" s="29">
         <v>6</v>
       </c>
-      <c r="H15" s="12"/>
-      <c r="J15" s="18"/>
+      <c r="H15" s="30"/>
+      <c r="J15" s="16"/>
     </row>
     <row r="16" spans="1:11" ht="66.599999999999994" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A16" s="16" t="s">
+      <c r="A16" s="28" t="s">
         <v>51</v>
       </c>
-      <c r="B16" s="7" t="s">
+      <c r="B16" s="29" t="s">
         <v>53</v>
       </c>
-      <c r="C16" s="7" t="s">
+      <c r="C16" s="29" t="s">
         <v>57</v>
       </c>
-      <c r="D16" s="7" t="s">
+      <c r="D16" s="29" t="s">
         <v>10</v>
       </c>
-      <c r="E16" s="7">
+      <c r="E16" s="29">
         <v>2</v>
       </c>
-      <c r="F16" s="7">
+      <c r="F16" s="29">
         <v>1</v>
       </c>
-      <c r="G16" s="7">
+      <c r="G16" s="29">
         <v>6</v>
       </c>
-      <c r="H16" s="12"/>
-      <c r="J16" s="11"/>
+      <c r="H16" s="30"/>
+      <c r="J16" s="10"/>
     </row>
     <row r="17" spans="1:10" ht="58.8" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A17" s="16" t="s">
+      <c r="A17" s="28" t="s">
         <v>52</v>
       </c>
-      <c r="B17" s="7" t="s">
+      <c r="B17" s="29" t="s">
         <v>54</v>
       </c>
-      <c r="C17" s="7" t="s">
+      <c r="C17" s="29" t="s">
         <v>57</v>
       </c>
-      <c r="D17" s="7" t="s">
+      <c r="D17" s="29" t="s">
         <v>10</v>
       </c>
-      <c r="E17" s="7">
+      <c r="E17" s="29">
         <v>2</v>
       </c>
-      <c r="F17" s="7">
+      <c r="F17" s="29">
         <v>1</v>
       </c>
-      <c r="G17" s="7">
+      <c r="G17" s="29">
         <v>6</v>
       </c>
-      <c r="H17" s="12"/>
+      <c r="H17" s="30"/>
     </row>
     <row r="18" spans="1:10" ht="54.6" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A18" s="15" t="s">
+      <c r="A18" s="13" t="s">
         <v>25</v>
       </c>
       <c r="B18" s="7" t="s">
@@ -1801,14 +1806,14 @@
       <c r="G18" s="7">
         <v>3</v>
       </c>
-      <c r="H18" s="12"/>
+      <c r="H18" s="11"/>
       <c r="I18" s="9"/>
     </row>
     <row r="19" spans="1:10" ht="63" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A19" s="16" t="s">
+      <c r="A19" s="14" t="s">
         <v>48</v>
       </c>
-      <c r="B19" s="21" t="s">
+      <c r="B19" s="19" t="s">
         <v>55</v>
       </c>
       <c r="C19" s="7" t="s">
@@ -1826,13 +1831,13 @@
       <c r="G19" s="7">
         <v>6</v>
       </c>
-      <c r="H19" s="12"/>
-      <c r="J19" s="24" t="s">
+      <c r="H19" s="11"/>
+      <c r="J19" s="20" t="s">
         <v>58</v>
       </c>
     </row>
     <row r="20" spans="1:10" ht="39.6" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A20" s="17" t="s">
+      <c r="A20" s="15" t="s">
         <v>31</v>
       </c>
       <c r="B20" s="8" t="s">
@@ -1853,7 +1858,7 @@
       <c r="G20" s="8">
         <v>33</v>
       </c>
-      <c r="H20" s="14"/>
+      <c r="H20" s="12"/>
     </row>
     <row r="21" spans="1:10" ht="32.4" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A21" s="1"/>

</xml_diff>